<commit_message>
Excel Check list change
</commit_message>
<xml_diff>
--- a/ShipStowage.xlsx
+++ b/ShipStowage.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\CLionProjects\ship-stowage-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71515662-A2BA-49C2-B347-A09271104284}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856A1A89-36A4-415A-8CEA-0998C55B1EC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="82">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -438,6 +438,9 @@
   </si>
   <si>
     <t>AbstractAlgorithm</t>
+  </si>
+  <si>
+    <t>v</t>
   </si>
 </sst>
 </file>
@@ -785,37 +788,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -835,6 +811,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -844,89 +886,61 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -1207,145 +1221,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6A2D0E-2C86-4ADB-83F2-CB80CC937DE8}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="54.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5" customWidth="1"/>
-    <col min="4" max="4" width="4.875" customWidth="1"/>
-    <col min="5" max="5" width="23.625" customWidth="1"/>
+    <col min="3" max="3" width="2.625" customWidth="1"/>
+    <col min="4" max="4" width="8.375" customWidth="1"/>
+    <col min="5" max="5" width="4.875" customWidth="1"/>
+    <col min="6" max="6" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="34" t="s">
+    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="34" t="s">
+      <c r="B1" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="C1" s="14"/>
+      <c r="E1" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="E1" s="37"/>
-      <c r="F1" s="38" t="s">
+      <c r="F1" s="27"/>
+      <c r="G1" s="16" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A2" s="35">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="39">
+      <c r="C2" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="17">
         <v>1</v>
       </c>
-      <c r="E2" s="42" t="s">
+      <c r="F2" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="45">
+      <c r="G2" s="23">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" x14ac:dyDescent="0.25">
-      <c r="A3" s="35" t="s">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D3" s="40">
+      <c r="C3" s="9"/>
+      <c r="E3" s="18">
         <v>2</v>
       </c>
-      <c r="E3" s="43" t="s">
+      <c r="F3" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="46">
+      <c r="G3" s="24">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="35" t="s">
+    <row r="4" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15" t="s">
         <v>60</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D4" s="41">
+      <c r="C4" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="19">
         <v>3</v>
       </c>
-      <c r="E4" s="44" t="s">
+      <c r="F4" s="22" t="s">
         <v>78</v>
       </c>
-      <c r="F4" s="47">
+      <c r="G4" s="25">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="35" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
         <v>62</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="35" t="s">
+      <c r="C5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="15" t="s">
         <v>64</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="35" t="s">
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="15" t="s">
         <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="35" t="s">
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
         <v>68</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="35" t="s">
+      <c r="C8" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="15" t="s">
         <v>70</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="15" t="s">
         <v>72</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="35" t="s">
+      <c r="C10" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>75</v>
       </c>
+      <c r="C11" s="9" t="s">
+        <v>81</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="E1:F1"/>
   </mergeCells>
+  <conditionalFormatting sqref="B2:B11">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>C2&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1353,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1366,49 +1410,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="E1" s="15" t="s">
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="E1" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="27"/>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="E2" s="19" t="s">
+      <c r="A2" s="28"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="E2" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="19"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="7" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="21"/>
-      <c r="F4" s="21"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="13" t="s">
         <v>24</v>
       </c>
       <c r="C5" s="2"/>
@@ -1419,294 +1463,293 @@
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="32" t="s">
+      <c r="B6" s="13" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="47" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="19"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="13" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="E7" s="30"/>
-      <c r="F7" s="20"/>
+      <c r="E7" s="48"/>
+      <c r="F7" s="33"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="12" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="20"/>
+      <c r="E8" s="48"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="12" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="20"/>
+      <c r="E9" s="48"/>
+      <c r="F9" s="33"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="13" t="s">
         <v>30</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="20"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="33"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="32" t="s">
+      <c r="B11" s="13" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="E11" s="30"/>
-      <c r="F11" s="20"/>
+      <c r="E11" s="48"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="22"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="12" t="s">
         <v>32</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="24"/>
+      <c r="F13" s="35"/>
     </row>
     <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="17" t="s">
+      <c r="B14" s="8" t="s">
         <v>33</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="35"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="13" t="s">
         <v>34</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="24"/>
+      <c r="E15" s="35"/>
+      <c r="F15" s="35"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="13" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
+      <c r="E16" s="35"/>
+      <c r="F16" s="35"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="13" t="s">
         <v>36</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="24"/>
+      <c r="E17" s="35"/>
+      <c r="F17" s="35"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="13" t="s">
         <v>37</v>
       </c>
       <c r="C18" s="2"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="13" t="s">
         <v>38</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="E19" s="28" t="s">
+      <c r="E19" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="24"/>
+      <c r="F19" s="35"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="13" t="s">
         <v>39</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="24"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="35"/>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="13" t="s">
         <v>40</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="24"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="35"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="13" t="s">
         <v>41</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="24"/>
+      <c r="E22" s="36"/>
+      <c r="F22" s="35"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="13" t="s">
         <v>42</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="24"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="35"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E24" s="13"/>
-      <c r="F24" s="13"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="33"/>
-      <c r="E25" s="25" t="s">
+      <c r="B25" s="29"/>
+      <c r="E25" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="25"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="E26" s="25"/>
-      <c r="F26" s="25"/>
+      <c r="B26" s="30"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="E27" s="25"/>
-      <c r="F27" s="25"/>
+      <c r="B27" s="31"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="D28" s="13"/>
+      <c r="B28" s="31"/>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D29" s="13"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D30" s="13"/>
-      <c r="G30" s="13"/>
+      <c r="D30" s="4"/>
+      <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="D31" s="13"/>
-      <c r="G31" s="13"/>
+      <c r="D31" s="4"/>
+      <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="13"/>
-      <c r="D32" s="13"/>
-      <c r="G32" s="13"/>
+      <c r="A32" s="3"/>
+      <c r="B32" s="4"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="G32" s="4"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" s="12"/>
-      <c r="B33" s="3" t="s">
+      <c r="A33" s="3"/>
+      <c r="B33" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-      <c r="G33" s="13"/>
+      <c r="C33" s="39"/>
+      <c r="D33" s="40"/>
+      <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="13"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="8"/>
-      <c r="G34" s="13"/>
+      <c r="A34" s="4"/>
+      <c r="B34" s="41"/>
+      <c r="C34" s="42"/>
+      <c r="D34" s="43"/>
+      <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="9"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="14"/>
-      <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="45"/>
+      <c r="D35" s="46"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A1:C2"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
-    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="B33:D35"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="E6:E11"/>
+    <mergeCell ref="E13:E17"/>
     <mergeCell ref="F2:F4"/>
     <mergeCell ref="F6:F11"/>
     <mergeCell ref="F13:F17"/>
@@ -1714,10 +1757,11 @@
     <mergeCell ref="E25:E27"/>
     <mergeCell ref="F19:F23"/>
     <mergeCell ref="F25:F27"/>
-    <mergeCell ref="B33:D35"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="E6:E11"/>
-    <mergeCell ref="E13:E17"/>
+    <mergeCell ref="A1:C2"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A28:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementing some of the algorithm validation checks in the algo cpp
</commit_message>
<xml_diff>
--- a/ShipStowage.xlsx
+++ b/ShipStowage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\CLionProjects\ship-stowage-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856A1A89-36A4-415A-8CEA-0998C55B1EC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5004E66-1AF1-495C-BABA-7995D34420BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pdf table of contents" sheetId="3" r:id="rId1"/>
@@ -865,6 +865,57 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -876,57 +927,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1223,8 +1223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A6A2D0E-2C86-4ADB-83F2-CB80CC937DE8}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1397,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1410,11 +1410,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
       <c r="E1" s="6" t="s">
         <v>45</v>
       </c>
@@ -1423,17 +1423,17 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="28"/>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28"/>
-      <c r="E2" s="32" t="s">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="E2" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="F2" s="32"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
     </row>
     <row r="4" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
@@ -1445,8 +1445,8 @@
       <c r="C4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
@@ -1467,10 +1467,10 @@
         <v>25</v>
       </c>
       <c r="C6" s="2"/>
-      <c r="E6" s="47" t="s">
+      <c r="E6" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="F6" s="32"/>
+      <c r="F6" s="37"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -1480,8 +1480,8 @@
         <v>26</v>
       </c>
       <c r="C7" s="2"/>
-      <c r="E7" s="48"/>
-      <c r="F7" s="33"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="38"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -1491,8 +1491,8 @@
         <v>27</v>
       </c>
       <c r="C8" s="2"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="33"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="38"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -1502,8 +1502,8 @@
         <v>28</v>
       </c>
       <c r="C9" s="2"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="33"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="38"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -1513,8 +1513,8 @@
         <v>30</v>
       </c>
       <c r="C10" s="2"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="33"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="38"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -1524,8 +1524,8 @@
         <v>29</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="33"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="38"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -1548,10 +1548,10 @@
         <v>32</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="E13" s="35" t="s">
+      <c r="E13" s="42" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="35"/>
+      <c r="F13" s="42"/>
     </row>
     <row r="14" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -1561,8 +1561,8 @@
         <v>33</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="E14" s="35"/>
-      <c r="F14" s="35"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -1572,8 +1572,8 @@
         <v>34</v>
       </c>
       <c r="C15" s="2"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -1583,8 +1583,8 @@
         <v>35</v>
       </c>
       <c r="C16" s="2"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -1594,8 +1594,8 @@
         <v>36</v>
       </c>
       <c r="C17" s="2"/>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -1616,10 +1616,10 @@
         <v>38</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="35"/>
+      <c r="F19" s="42"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
@@ -1629,8 +1629,8 @@
         <v>39</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="35"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="42"/>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -1640,8 +1640,8 @@
         <v>40</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="35"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="42"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -1651,8 +1651,8 @@
         <v>41</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="E22" s="36"/>
-      <c r="F22" s="35"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="42"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -1662,44 +1662,44 @@
         <v>42</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="35"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="42"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="E25" s="37" t="s">
+      <c r="B25" s="46"/>
+      <c r="E25" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="F25" s="37"/>
+      <c r="F25" s="44"/>
     </row>
     <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.25">
-      <c r="A26" s="30" t="s">
+      <c r="A26" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="30"/>
-      <c r="E26" s="37"/>
-      <c r="F26" s="37"/>
+      <c r="B26" s="47"/>
+      <c r="E26" s="44"/>
+      <c r="F26" s="44"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="48" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="E27" s="37"/>
-      <c r="F27" s="37"/>
+      <c r="B27" s="48"/>
+      <c r="E27" s="44"/>
+      <c r="F27" s="44"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B28" s="31"/>
+      <c r="B28" s="48"/>
       <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1722,24 +1722,24 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="3"/>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="28" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="39"/>
-      <c r="D33" s="40"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
-      <c r="B34" s="41"/>
-      <c r="C34" s="42"/>
-      <c r="D34" s="43"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="33"/>
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="44"/>
-      <c r="C35" s="45"/>
-      <c r="D35" s="46"/>
+      <c r="B35" s="34"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="36"/>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>

</xml_diff>

<commit_message>
Adding the algorithm registrar
</commit_message>
<xml_diff>
--- a/ShipStowage.xlsx
+++ b/ShipStowage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Allen\CLionProjects\ship-stowage-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5004E66-1AF1-495C-BABA-7995D34420BE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE71D7D0-34A5-49E2-B0FB-6D3D7D814175}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1224,7 +1224,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C11"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1397,8 +1397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>